<commit_message>
add the lifting events
</commit_message>
<xml_diff>
--- a/Germany_NPIs.xlsx
+++ b/Germany_NPIs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liuqi\Desktop\old_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liuqi\Desktop\SEIR-master\SEIR-master\DataCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BF055B-5D87-4286-891A-9B64B57BCB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDAACDC-9372-4F33-A53F-B4AB17E32FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5060" yWindow="840" windowWidth="10060" windowHeight="9080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1037" windowWidth="18711" windowHeight="10903" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,74 +63,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -150,7 +82,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CCE8CF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -407,13 +339,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1">
         <v>0</v>
       </c>
@@ -421,7 +353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -429,7 +361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>0</v>
       </c>
@@ -437,7 +369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>0</v>
       </c>
@@ -445,7 +377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>0</v>
       </c>
@@ -453,7 +385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>0</v>
       </c>
@@ -461,7 +393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>0</v>
       </c>
@@ -469,7 +401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -477,7 +409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>0</v>
       </c>
@@ -485,7 +417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>0</v>
       </c>
@@ -493,7 +425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>0</v>
       </c>
@@ -501,7 +433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>0</v>
       </c>
@@ -509,7 +441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>1</v>
       </c>
@@ -517,7 +449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>0</v>
       </c>
@@ -525,7 +457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>0</v>
       </c>
@@ -533,7 +465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>1</v>
       </c>
@@ -541,7 +473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>0</v>
       </c>
@@ -549,7 +481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>0</v>
       </c>
@@ -557,7 +489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>0</v>
       </c>
@@ -565,7 +497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>0</v>
       </c>
@@ -573,7 +505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>0</v>
       </c>
@@ -581,7 +513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>1</v>
       </c>
@@ -589,7 +521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>0</v>
       </c>
@@ -597,7 +529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>0</v>
       </c>
@@ -605,7 +537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>0</v>
       </c>
@@ -613,7 +545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>0</v>
       </c>
@@ -621,7 +553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>0</v>
       </c>
@@ -629,7 +561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>0</v>
       </c>
@@ -637,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>0</v>
       </c>
@@ -645,7 +577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>0</v>
       </c>
@@ -653,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>1</v>
       </c>
@@ -661,7 +593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>0</v>
       </c>
@@ -669,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>0</v>
       </c>
@@ -677,7 +609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>0</v>
       </c>
@@ -685,7 +617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>0</v>
       </c>
@@ -693,7 +625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>0</v>
       </c>
@@ -701,7 +633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>0</v>
       </c>
@@ -709,7 +641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>0</v>
       </c>
@@ -717,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>0</v>
       </c>
@@ -725,7 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>0</v>
       </c>
@@ -733,7 +665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>0</v>
       </c>
@@ -741,7 +673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>0</v>
       </c>
@@ -749,7 +681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>0</v>
       </c>
@@ -757,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>0</v>
       </c>
@@ -765,7 +697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>0</v>
       </c>
@@ -773,7 +705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>0</v>
       </c>
@@ -781,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>0</v>
       </c>
@@ -789,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>0</v>
       </c>
@@ -797,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>0</v>
       </c>
@@ -805,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>0</v>
       </c>
@@ -813,15 +745,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>0</v>
       </c>
@@ -829,7 +761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>0</v>
       </c>
@@ -837,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>0</v>
       </c>
@@ -845,7 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>0</v>
       </c>
@@ -853,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>0</v>
       </c>
@@ -861,7 +793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>0</v>
       </c>
@@ -869,7 +801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>0</v>
       </c>
@@ -877,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>0</v>
       </c>
@@ -885,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>0</v>
       </c>
@@ -893,15 +825,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B61">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>0</v>
       </c>
@@ -909,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>0</v>
       </c>
@@ -917,7 +849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>0</v>
       </c>
@@ -925,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>0</v>
       </c>
@@ -933,7 +865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>0</v>
       </c>
@@ -941,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>0</v>
       </c>
@@ -949,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>0</v>
       </c>
@@ -957,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>0</v>
       </c>
@@ -965,7 +897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>0</v>
       </c>
@@ -973,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>0</v>
       </c>
@@ -981,7 +913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>0</v>
       </c>
@@ -989,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>0</v>
       </c>
@@ -997,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>0</v>
       </c>
@@ -1005,7 +937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>0</v>
       </c>
@@ -1013,15 +945,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A76">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B76">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>0</v>
       </c>
@@ -1029,7 +961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>0</v>
       </c>
@@ -1037,7 +969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>0</v>
       </c>
@@ -1045,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>0</v>
       </c>
@@ -1053,7 +985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>0</v>
       </c>
@@ -1061,7 +993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>0</v>
       </c>
@@ -1069,7 +1001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>0</v>
       </c>
@@ -1077,7 +1009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>0</v>
       </c>
@@ -1085,7 +1017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>0</v>
       </c>
@@ -1093,7 +1025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>0</v>
       </c>
@@ -1101,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A87">
         <v>0</v>
       </c>
@@ -1109,7 +1041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A88">
         <v>0</v>
       </c>
@@ -1117,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A89">
         <v>0</v>
       </c>
@@ -1125,7 +1057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A90">
         <v>0</v>
       </c>
@@ -1133,7 +1065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A91">
         <v>0</v>
       </c>
@@ -1141,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A92">
         <v>0</v>
       </c>

</xml_diff>